<commit_message>
building function to read all stock prices in NASDAQ
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Python Scripts\Deepdive-on-Regular-Investing-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2DFBAFD-320A-40C8-AE9B-D80B017E69F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A656D73-B228-46BE-B786-CDE8CE4533CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{945109A7-FE98-44CC-ACDC-346516250C59}"/>
+    <workbookView xWindow="9765" yWindow="0" windowWidth="18870" windowHeight="15600" xr2:uid="{945109A7-FE98-44CC-ACDC-346516250C59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB92B57-5725-4BAD-A9D0-933ACE92FF11}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,13 +1075,13 @@
     </row>
     <row r="16" spans="1:25" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="B16" s="3">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C16" s="3">
-        <v>-10400</v>
+        <v>-100</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F16" s="6">
         <f>FV(A16,B16,C16,D16,E16)</f>
-        <v>70120.764999999956</v>
+        <v>9001.6409272408928</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>

</xml_diff>